<commit_message>
Cập nhật báo cáo tuần của Thành
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Thanh.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Thanh.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Task_Guideline" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn__FilterDatabase">Task!$A$5:$F$11</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Task!$A$1:$N$32</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase">Task!$A$6:$F$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Task!$A$1:$N$33</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
   <si>
     <t>Project</t>
   </si>
@@ -390,6 +390,32 @@
   </si>
   <si>
     <t>Hoàn thành: chỉnh "Admin" thành "Thủ thư" ở các chức năng 9 và 10.</t>
+  </si>
+  <si>
+    <t>27/9/2012</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa và hoàn thiện SRS</t>
+  </si>
+  <si>
+    <t>Họp nhóm xác 
+định project</t>
+  </si>
+  <si>
+    <t>các chức năng cơ bản được 
+xác định</t>
+  </si>
+  <si>
+    <t>Hoàn Thành</t>
+  </si>
+  <si>
+    <t>Cả nhóm</t>
+  </si>
+  <si>
+    <t>Viết SDD các phần chức năng như SRS</t>
+  </si>
+  <si>
+    <t>1 phần SDD</t>
   </si>
 </sst>
 </file>
@@ -535,7 +561,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -580,6 +606,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3103,10 +3132,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ24"/>
+  <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3233,24 +3262,28 @@
       </c>
     </row>
     <row r="4" spans="1:1024" s="12" customFormat="1">
-      <c r="A4" s="8" t="s">
-        <v>35</v>
+      <c r="A4" s="8">
+        <v>41099</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="D4" s="10" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E4" s="9">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F4" s="9">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="H4" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
@@ -4268,24 +4301,22 @@
       <c r="AMI4" s="11"/>
       <c r="AMJ4" s="11"/>
     </row>
-    <row r="5" spans="1:1024" s="12" customFormat="1" ht="85.5">
+    <row r="5" spans="1:1024" s="12" customFormat="1">
       <c r="A5" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="C5" s="9"/>
       <c r="D5" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="9">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F5" s="9">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -5306,24 +5337,24 @@
       <c r="AMI5" s="11"/>
       <c r="AMJ5" s="11"/>
     </row>
-    <row r="6" spans="1:1024" s="12" customFormat="1" ht="42.75">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:1024" s="12" customFormat="1" ht="85.5">
+      <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>41</v>
+      <c r="D6" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="E6" s="9">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F6" s="9">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -6344,13 +6375,25 @@
       <c r="AMI6" s="11"/>
       <c r="AMJ6" s="11"/>
     </row>
-    <row r="7" spans="1:1024" s="12" customFormat="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+    <row r="7" spans="1:1024" s="12" customFormat="1" ht="42.75">
+      <c r="A7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.5</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -6360,20 +6403,20 @@
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="11"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="11"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
       <c r="AD7" s="11"/>
       <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
@@ -7371,12 +7414,24 @@
       <c r="AMJ7" s="11"/>
     </row>
     <row r="8" spans="1:1024" s="12" customFormat="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="A8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2</v>
+      </c>
+      <c r="F8" s="9">
+        <v>2</v>
+      </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -7386,20 +7441,20 @@
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
       <c r="AD8" s="11"/>
       <c r="AE8" s="11"/>
       <c r="AF8" s="11"/>
@@ -8396,12 +8451,20 @@
       <c r="AMI8" s="11"/>
       <c r="AMJ8" s="11"/>
     </row>
-    <row r="9" spans="1:1024" s="12" customFormat="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+    <row r="9" spans="1:1024" s="12" customFormat="1" ht="28.5">
+      <c r="A9" s="15">
+        <v>40918</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="E9" s="9">
+        <v>4</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -24812,6 +24875,1032 @@
       <c r="AMI24" s="11"/>
       <c r="AMJ24" s="11"/>
     </row>
+    <row r="25" spans="1:1024" s="12" customFormat="1">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+      <c r="AE25" s="11"/>
+      <c r="AF25" s="11"/>
+      <c r="AG25" s="11"/>
+      <c r="AH25" s="11"/>
+      <c r="AI25" s="11"/>
+      <c r="AJ25" s="11"/>
+      <c r="AK25" s="11"/>
+      <c r="AL25" s="11"/>
+      <c r="AM25" s="11"/>
+      <c r="AN25" s="11"/>
+      <c r="AO25" s="11"/>
+      <c r="AP25" s="11"/>
+      <c r="AQ25" s="11"/>
+      <c r="AR25" s="11"/>
+      <c r="AS25" s="11"/>
+      <c r="AT25" s="11"/>
+      <c r="AU25" s="11"/>
+      <c r="AV25" s="11"/>
+      <c r="AW25" s="11"/>
+      <c r="AX25" s="11"/>
+      <c r="AY25" s="11"/>
+      <c r="AZ25" s="11"/>
+      <c r="BA25" s="11"/>
+      <c r="BB25" s="11"/>
+      <c r="BC25" s="11"/>
+      <c r="BD25" s="11"/>
+      <c r="BE25" s="11"/>
+      <c r="BF25" s="11"/>
+      <c r="BG25" s="11"/>
+      <c r="BH25" s="11"/>
+      <c r="BI25" s="11"/>
+      <c r="BJ25" s="11"/>
+      <c r="BK25" s="11"/>
+      <c r="BL25" s="11"/>
+      <c r="BM25" s="11"/>
+      <c r="BN25" s="11"/>
+      <c r="BO25" s="11"/>
+      <c r="BP25" s="11"/>
+      <c r="BQ25" s="11"/>
+      <c r="BR25" s="11"/>
+      <c r="BS25" s="11"/>
+      <c r="BT25" s="11"/>
+      <c r="BU25" s="11"/>
+      <c r="BV25" s="11"/>
+      <c r="BW25" s="11"/>
+      <c r="BX25" s="11"/>
+      <c r="BY25" s="11"/>
+      <c r="BZ25" s="11"/>
+      <c r="CA25" s="11"/>
+      <c r="CB25" s="11"/>
+      <c r="CC25" s="11"/>
+      <c r="CD25" s="11"/>
+      <c r="CE25" s="11"/>
+      <c r="CF25" s="11"/>
+      <c r="CG25" s="11"/>
+      <c r="CH25" s="11"/>
+      <c r="CI25" s="11"/>
+      <c r="CJ25" s="11"/>
+      <c r="CK25" s="11"/>
+      <c r="CL25" s="11"/>
+      <c r="CM25" s="11"/>
+      <c r="CN25" s="11"/>
+      <c r="CO25" s="11"/>
+      <c r="CP25" s="11"/>
+      <c r="CQ25" s="11"/>
+      <c r="CR25" s="11"/>
+      <c r="CS25" s="11"/>
+      <c r="CT25" s="11"/>
+      <c r="CU25" s="11"/>
+      <c r="CV25" s="11"/>
+      <c r="CW25" s="11"/>
+      <c r="CX25" s="11"/>
+      <c r="CY25" s="11"/>
+      <c r="CZ25" s="11"/>
+      <c r="DA25" s="11"/>
+      <c r="DB25" s="11"/>
+      <c r="DC25" s="11"/>
+      <c r="DD25" s="11"/>
+      <c r="DE25" s="11"/>
+      <c r="DF25" s="11"/>
+      <c r="DG25" s="11"/>
+      <c r="DH25" s="11"/>
+      <c r="DI25" s="11"/>
+      <c r="DJ25" s="11"/>
+      <c r="DK25" s="11"/>
+      <c r="DL25" s="11"/>
+      <c r="DM25" s="11"/>
+      <c r="DN25" s="11"/>
+      <c r="DO25" s="11"/>
+      <c r="DP25" s="11"/>
+      <c r="DQ25" s="11"/>
+      <c r="DR25" s="11"/>
+      <c r="DS25" s="11"/>
+      <c r="DT25" s="11"/>
+      <c r="DU25" s="11"/>
+      <c r="DV25" s="11"/>
+      <c r="DW25" s="11"/>
+      <c r="DX25" s="11"/>
+      <c r="DY25" s="11"/>
+      <c r="DZ25" s="11"/>
+      <c r="EA25" s="11"/>
+      <c r="EB25" s="11"/>
+      <c r="EC25" s="11"/>
+      <c r="ED25" s="11"/>
+      <c r="EE25" s="11"/>
+      <c r="EF25" s="11"/>
+      <c r="EG25" s="11"/>
+      <c r="EH25" s="11"/>
+      <c r="EI25" s="11"/>
+      <c r="EJ25" s="11"/>
+      <c r="EK25" s="11"/>
+      <c r="EL25" s="11"/>
+      <c r="EM25" s="11"/>
+      <c r="EN25" s="11"/>
+      <c r="EO25" s="11"/>
+      <c r="EP25" s="11"/>
+      <c r="EQ25" s="11"/>
+      <c r="ER25" s="11"/>
+      <c r="ES25" s="11"/>
+      <c r="ET25" s="11"/>
+      <c r="EU25" s="11"/>
+      <c r="EV25" s="11"/>
+      <c r="EW25" s="11"/>
+      <c r="EX25" s="11"/>
+      <c r="EY25" s="11"/>
+      <c r="EZ25" s="11"/>
+      <c r="FA25" s="11"/>
+      <c r="FB25" s="11"/>
+      <c r="FC25" s="11"/>
+      <c r="FD25" s="11"/>
+      <c r="FE25" s="11"/>
+      <c r="FF25" s="11"/>
+      <c r="FG25" s="11"/>
+      <c r="FH25" s="11"/>
+      <c r="FI25" s="11"/>
+      <c r="FJ25" s="11"/>
+      <c r="FK25" s="11"/>
+      <c r="FL25" s="11"/>
+      <c r="FM25" s="11"/>
+      <c r="FN25" s="11"/>
+      <c r="FO25" s="11"/>
+      <c r="FP25" s="11"/>
+      <c r="FQ25" s="11"/>
+      <c r="FR25" s="11"/>
+      <c r="FS25" s="11"/>
+      <c r="FT25" s="11"/>
+      <c r="FU25" s="11"/>
+      <c r="FV25" s="11"/>
+      <c r="FW25" s="11"/>
+      <c r="FX25" s="11"/>
+      <c r="FY25" s="11"/>
+      <c r="FZ25" s="11"/>
+      <c r="GA25" s="11"/>
+      <c r="GB25" s="11"/>
+      <c r="GC25" s="11"/>
+      <c r="GD25" s="11"/>
+      <c r="GE25" s="11"/>
+      <c r="GF25" s="11"/>
+      <c r="GG25" s="11"/>
+      <c r="GH25" s="11"/>
+      <c r="GI25" s="11"/>
+      <c r="GJ25" s="11"/>
+      <c r="GK25" s="11"/>
+      <c r="GL25" s="11"/>
+      <c r="GM25" s="11"/>
+      <c r="GN25" s="11"/>
+      <c r="GO25" s="11"/>
+      <c r="GP25" s="11"/>
+      <c r="GQ25" s="11"/>
+      <c r="GR25" s="11"/>
+      <c r="GS25" s="11"/>
+      <c r="GT25" s="11"/>
+      <c r="GU25" s="11"/>
+      <c r="GV25" s="11"/>
+      <c r="GW25" s="11"/>
+      <c r="GX25" s="11"/>
+      <c r="GY25" s="11"/>
+      <c r="GZ25" s="11"/>
+      <c r="HA25" s="11"/>
+      <c r="HB25" s="11"/>
+      <c r="HC25" s="11"/>
+      <c r="HD25" s="11"/>
+      <c r="HE25" s="11"/>
+      <c r="HF25" s="11"/>
+      <c r="HG25" s="11"/>
+      <c r="HH25" s="11"/>
+      <c r="HI25" s="11"/>
+      <c r="HJ25" s="11"/>
+      <c r="HK25" s="11"/>
+      <c r="HL25" s="11"/>
+      <c r="HM25" s="11"/>
+      <c r="HN25" s="11"/>
+      <c r="HO25" s="11"/>
+      <c r="HP25" s="11"/>
+      <c r="HQ25" s="11"/>
+      <c r="HR25" s="11"/>
+      <c r="HS25" s="11"/>
+      <c r="HT25" s="11"/>
+      <c r="HU25" s="11"/>
+      <c r="HV25" s="11"/>
+      <c r="HW25" s="11"/>
+      <c r="HX25" s="11"/>
+      <c r="HY25" s="11"/>
+      <c r="HZ25" s="11"/>
+      <c r="IA25" s="11"/>
+      <c r="IB25" s="11"/>
+      <c r="IC25" s="11"/>
+      <c r="ID25" s="11"/>
+      <c r="IE25" s="11"/>
+      <c r="IF25" s="11"/>
+      <c r="IG25" s="11"/>
+      <c r="IH25" s="11"/>
+      <c r="II25" s="11"/>
+      <c r="IJ25" s="11"/>
+      <c r="IK25" s="11"/>
+      <c r="IL25" s="11"/>
+      <c r="IM25" s="11"/>
+      <c r="IN25" s="11"/>
+      <c r="IO25" s="11"/>
+      <c r="IP25" s="11"/>
+      <c r="IQ25" s="11"/>
+      <c r="IR25" s="11"/>
+      <c r="IS25" s="11"/>
+      <c r="IT25" s="11"/>
+      <c r="IU25" s="11"/>
+      <c r="IV25" s="11"/>
+      <c r="IW25" s="11"/>
+      <c r="IX25" s="11"/>
+      <c r="IY25" s="11"/>
+      <c r="IZ25" s="11"/>
+      <c r="JA25" s="11"/>
+      <c r="JB25" s="11"/>
+      <c r="JC25" s="11"/>
+      <c r="JD25" s="11"/>
+      <c r="JE25" s="11"/>
+      <c r="JF25" s="11"/>
+      <c r="JG25" s="11"/>
+      <c r="JH25" s="11"/>
+      <c r="JI25" s="11"/>
+      <c r="JJ25" s="11"/>
+      <c r="JK25" s="11"/>
+      <c r="JL25" s="11"/>
+      <c r="JM25" s="11"/>
+      <c r="JN25" s="11"/>
+      <c r="JO25" s="11"/>
+      <c r="JP25" s="11"/>
+      <c r="JQ25" s="11"/>
+      <c r="JR25" s="11"/>
+      <c r="JS25" s="11"/>
+      <c r="JT25" s="11"/>
+      <c r="JU25" s="11"/>
+      <c r="JV25" s="11"/>
+      <c r="JW25" s="11"/>
+      <c r="JX25" s="11"/>
+      <c r="JY25" s="11"/>
+      <c r="JZ25" s="11"/>
+      <c r="KA25" s="11"/>
+      <c r="KB25" s="11"/>
+      <c r="KC25" s="11"/>
+      <c r="KD25" s="11"/>
+      <c r="KE25" s="11"/>
+      <c r="KF25" s="11"/>
+      <c r="KG25" s="11"/>
+      <c r="KH25" s="11"/>
+      <c r="KI25" s="11"/>
+      <c r="KJ25" s="11"/>
+      <c r="KK25" s="11"/>
+      <c r="KL25" s="11"/>
+      <c r="KM25" s="11"/>
+      <c r="KN25" s="11"/>
+      <c r="KO25" s="11"/>
+      <c r="KP25" s="11"/>
+      <c r="KQ25" s="11"/>
+      <c r="KR25" s="11"/>
+      <c r="KS25" s="11"/>
+      <c r="KT25" s="11"/>
+      <c r="KU25" s="11"/>
+      <c r="KV25" s="11"/>
+      <c r="KW25" s="11"/>
+      <c r="KX25" s="11"/>
+      <c r="KY25" s="11"/>
+      <c r="KZ25" s="11"/>
+      <c r="LA25" s="11"/>
+      <c r="LB25" s="11"/>
+      <c r="LC25" s="11"/>
+      <c r="LD25" s="11"/>
+      <c r="LE25" s="11"/>
+      <c r="LF25" s="11"/>
+      <c r="LG25" s="11"/>
+      <c r="LH25" s="11"/>
+      <c r="LI25" s="11"/>
+      <c r="LJ25" s="11"/>
+      <c r="LK25" s="11"/>
+      <c r="LL25" s="11"/>
+      <c r="LM25" s="11"/>
+      <c r="LN25" s="11"/>
+      <c r="LO25" s="11"/>
+      <c r="LP25" s="11"/>
+      <c r="LQ25" s="11"/>
+      <c r="LR25" s="11"/>
+      <c r="LS25" s="11"/>
+      <c r="LT25" s="11"/>
+      <c r="LU25" s="11"/>
+      <c r="LV25" s="11"/>
+      <c r="LW25" s="11"/>
+      <c r="LX25" s="11"/>
+      <c r="LY25" s="11"/>
+      <c r="LZ25" s="11"/>
+      <c r="MA25" s="11"/>
+      <c r="MB25" s="11"/>
+      <c r="MC25" s="11"/>
+      <c r="MD25" s="11"/>
+      <c r="ME25" s="11"/>
+      <c r="MF25" s="11"/>
+      <c r="MG25" s="11"/>
+      <c r="MH25" s="11"/>
+      <c r="MI25" s="11"/>
+      <c r="MJ25" s="11"/>
+      <c r="MK25" s="11"/>
+      <c r="ML25" s="11"/>
+      <c r="MM25" s="11"/>
+      <c r="MN25" s="11"/>
+      <c r="MO25" s="11"/>
+      <c r="MP25" s="11"/>
+      <c r="MQ25" s="11"/>
+      <c r="MR25" s="11"/>
+      <c r="MS25" s="11"/>
+      <c r="MT25" s="11"/>
+      <c r="MU25" s="11"/>
+      <c r="MV25" s="11"/>
+      <c r="MW25" s="11"/>
+      <c r="MX25" s="11"/>
+      <c r="MY25" s="11"/>
+      <c r="MZ25" s="11"/>
+      <c r="NA25" s="11"/>
+      <c r="NB25" s="11"/>
+      <c r="NC25" s="11"/>
+      <c r="ND25" s="11"/>
+      <c r="NE25" s="11"/>
+      <c r="NF25" s="11"/>
+      <c r="NG25" s="11"/>
+      <c r="NH25" s="11"/>
+      <c r="NI25" s="11"/>
+      <c r="NJ25" s="11"/>
+      <c r="NK25" s="11"/>
+      <c r="NL25" s="11"/>
+      <c r="NM25" s="11"/>
+      <c r="NN25" s="11"/>
+      <c r="NO25" s="11"/>
+      <c r="NP25" s="11"/>
+      <c r="NQ25" s="11"/>
+      <c r="NR25" s="11"/>
+      <c r="NS25" s="11"/>
+      <c r="NT25" s="11"/>
+      <c r="NU25" s="11"/>
+      <c r="NV25" s="11"/>
+      <c r="NW25" s="11"/>
+      <c r="NX25" s="11"/>
+      <c r="NY25" s="11"/>
+      <c r="NZ25" s="11"/>
+      <c r="OA25" s="11"/>
+      <c r="OB25" s="11"/>
+      <c r="OC25" s="11"/>
+      <c r="OD25" s="11"/>
+      <c r="OE25" s="11"/>
+      <c r="OF25" s="11"/>
+      <c r="OG25" s="11"/>
+      <c r="OH25" s="11"/>
+      <c r="OI25" s="11"/>
+      <c r="OJ25" s="11"/>
+      <c r="OK25" s="11"/>
+      <c r="OL25" s="11"/>
+      <c r="OM25" s="11"/>
+      <c r="ON25" s="11"/>
+      <c r="OO25" s="11"/>
+      <c r="OP25" s="11"/>
+      <c r="OQ25" s="11"/>
+      <c r="OR25" s="11"/>
+      <c r="OS25" s="11"/>
+      <c r="OT25" s="11"/>
+      <c r="OU25" s="11"/>
+      <c r="OV25" s="11"/>
+      <c r="OW25" s="11"/>
+      <c r="OX25" s="11"/>
+      <c r="OY25" s="11"/>
+      <c r="OZ25" s="11"/>
+      <c r="PA25" s="11"/>
+      <c r="PB25" s="11"/>
+      <c r="PC25" s="11"/>
+      <c r="PD25" s="11"/>
+      <c r="PE25" s="11"/>
+      <c r="PF25" s="11"/>
+      <c r="PG25" s="11"/>
+      <c r="PH25" s="11"/>
+      <c r="PI25" s="11"/>
+      <c r="PJ25" s="11"/>
+      <c r="PK25" s="11"/>
+      <c r="PL25" s="11"/>
+      <c r="PM25" s="11"/>
+      <c r="PN25" s="11"/>
+      <c r="PO25" s="11"/>
+      <c r="PP25" s="11"/>
+      <c r="PQ25" s="11"/>
+      <c r="PR25" s="11"/>
+      <c r="PS25" s="11"/>
+      <c r="PT25" s="11"/>
+      <c r="PU25" s="11"/>
+      <c r="PV25" s="11"/>
+      <c r="PW25" s="11"/>
+      <c r="PX25" s="11"/>
+      <c r="PY25" s="11"/>
+      <c r="PZ25" s="11"/>
+      <c r="QA25" s="11"/>
+      <c r="QB25" s="11"/>
+      <c r="QC25" s="11"/>
+      <c r="QD25" s="11"/>
+      <c r="QE25" s="11"/>
+      <c r="QF25" s="11"/>
+      <c r="QG25" s="11"/>
+      <c r="QH25" s="11"/>
+      <c r="QI25" s="11"/>
+      <c r="QJ25" s="11"/>
+      <c r="QK25" s="11"/>
+      <c r="QL25" s="11"/>
+      <c r="QM25" s="11"/>
+      <c r="QN25" s="11"/>
+      <c r="QO25" s="11"/>
+      <c r="QP25" s="11"/>
+      <c r="QQ25" s="11"/>
+      <c r="QR25" s="11"/>
+      <c r="QS25" s="11"/>
+      <c r="QT25" s="11"/>
+      <c r="QU25" s="11"/>
+      <c r="QV25" s="11"/>
+      <c r="QW25" s="11"/>
+      <c r="QX25" s="11"/>
+      <c r="QY25" s="11"/>
+      <c r="QZ25" s="11"/>
+      <c r="RA25" s="11"/>
+      <c r="RB25" s="11"/>
+      <c r="RC25" s="11"/>
+      <c r="RD25" s="11"/>
+      <c r="RE25" s="11"/>
+      <c r="RF25" s="11"/>
+      <c r="RG25" s="11"/>
+      <c r="RH25" s="11"/>
+      <c r="RI25" s="11"/>
+      <c r="RJ25" s="11"/>
+      <c r="RK25" s="11"/>
+      <c r="RL25" s="11"/>
+      <c r="RM25" s="11"/>
+      <c r="RN25" s="11"/>
+      <c r="RO25" s="11"/>
+      <c r="RP25" s="11"/>
+      <c r="RQ25" s="11"/>
+      <c r="RR25" s="11"/>
+      <c r="RS25" s="11"/>
+      <c r="RT25" s="11"/>
+      <c r="RU25" s="11"/>
+      <c r="RV25" s="11"/>
+      <c r="RW25" s="11"/>
+      <c r="RX25" s="11"/>
+      <c r="RY25" s="11"/>
+      <c r="RZ25" s="11"/>
+      <c r="SA25" s="11"/>
+      <c r="SB25" s="11"/>
+      <c r="SC25" s="11"/>
+      <c r="SD25" s="11"/>
+      <c r="SE25" s="11"/>
+      <c r="SF25" s="11"/>
+      <c r="SG25" s="11"/>
+      <c r="SH25" s="11"/>
+      <c r="SI25" s="11"/>
+      <c r="SJ25" s="11"/>
+      <c r="SK25" s="11"/>
+      <c r="SL25" s="11"/>
+      <c r="SM25" s="11"/>
+      <c r="SN25" s="11"/>
+      <c r="SO25" s="11"/>
+      <c r="SP25" s="11"/>
+      <c r="SQ25" s="11"/>
+      <c r="SR25" s="11"/>
+      <c r="SS25" s="11"/>
+      <c r="ST25" s="11"/>
+      <c r="SU25" s="11"/>
+      <c r="SV25" s="11"/>
+      <c r="SW25" s="11"/>
+      <c r="SX25" s="11"/>
+      <c r="SY25" s="11"/>
+      <c r="SZ25" s="11"/>
+      <c r="TA25" s="11"/>
+      <c r="TB25" s="11"/>
+      <c r="TC25" s="11"/>
+      <c r="TD25" s="11"/>
+      <c r="TE25" s="11"/>
+      <c r="TF25" s="11"/>
+      <c r="TG25" s="11"/>
+      <c r="TH25" s="11"/>
+      <c r="TI25" s="11"/>
+      <c r="TJ25" s="11"/>
+      <c r="TK25" s="11"/>
+      <c r="TL25" s="11"/>
+      <c r="TM25" s="11"/>
+      <c r="TN25" s="11"/>
+      <c r="TO25" s="11"/>
+      <c r="TP25" s="11"/>
+      <c r="TQ25" s="11"/>
+      <c r="TR25" s="11"/>
+      <c r="TS25" s="11"/>
+      <c r="TT25" s="11"/>
+      <c r="TU25" s="11"/>
+      <c r="TV25" s="11"/>
+      <c r="TW25" s="11"/>
+      <c r="TX25" s="11"/>
+      <c r="TY25" s="11"/>
+      <c r="TZ25" s="11"/>
+      <c r="UA25" s="11"/>
+      <c r="UB25" s="11"/>
+      <c r="UC25" s="11"/>
+      <c r="UD25" s="11"/>
+      <c r="UE25" s="11"/>
+      <c r="UF25" s="11"/>
+      <c r="UG25" s="11"/>
+      <c r="UH25" s="11"/>
+      <c r="UI25" s="11"/>
+      <c r="UJ25" s="11"/>
+      <c r="UK25" s="11"/>
+      <c r="UL25" s="11"/>
+      <c r="UM25" s="11"/>
+      <c r="UN25" s="11"/>
+      <c r="UO25" s="11"/>
+      <c r="UP25" s="11"/>
+      <c r="UQ25" s="11"/>
+      <c r="UR25" s="11"/>
+      <c r="US25" s="11"/>
+      <c r="UT25" s="11"/>
+      <c r="UU25" s="11"/>
+      <c r="UV25" s="11"/>
+      <c r="UW25" s="11"/>
+      <c r="UX25" s="11"/>
+      <c r="UY25" s="11"/>
+      <c r="UZ25" s="11"/>
+      <c r="VA25" s="11"/>
+      <c r="VB25" s="11"/>
+      <c r="VC25" s="11"/>
+      <c r="VD25" s="11"/>
+      <c r="VE25" s="11"/>
+      <c r="VF25" s="11"/>
+      <c r="VG25" s="11"/>
+      <c r="VH25" s="11"/>
+      <c r="VI25" s="11"/>
+      <c r="VJ25" s="11"/>
+      <c r="VK25" s="11"/>
+      <c r="VL25" s="11"/>
+      <c r="VM25" s="11"/>
+      <c r="VN25" s="11"/>
+      <c r="VO25" s="11"/>
+      <c r="VP25" s="11"/>
+      <c r="VQ25" s="11"/>
+      <c r="VR25" s="11"/>
+      <c r="VS25" s="11"/>
+      <c r="VT25" s="11"/>
+      <c r="VU25" s="11"/>
+      <c r="VV25" s="11"/>
+      <c r="VW25" s="11"/>
+      <c r="VX25" s="11"/>
+      <c r="VY25" s="11"/>
+      <c r="VZ25" s="11"/>
+      <c r="WA25" s="11"/>
+      <c r="WB25" s="11"/>
+      <c r="WC25" s="11"/>
+      <c r="WD25" s="11"/>
+      <c r="WE25" s="11"/>
+      <c r="WF25" s="11"/>
+      <c r="WG25" s="11"/>
+      <c r="WH25" s="11"/>
+      <c r="WI25" s="11"/>
+      <c r="WJ25" s="11"/>
+      <c r="WK25" s="11"/>
+      <c r="WL25" s="11"/>
+      <c r="WM25" s="11"/>
+      <c r="WN25" s="11"/>
+      <c r="WO25" s="11"/>
+      <c r="WP25" s="11"/>
+      <c r="WQ25" s="11"/>
+      <c r="WR25" s="11"/>
+      <c r="WS25" s="11"/>
+      <c r="WT25" s="11"/>
+      <c r="WU25" s="11"/>
+      <c r="WV25" s="11"/>
+      <c r="WW25" s="11"/>
+      <c r="WX25" s="11"/>
+      <c r="WY25" s="11"/>
+      <c r="WZ25" s="11"/>
+      <c r="XA25" s="11"/>
+      <c r="XB25" s="11"/>
+      <c r="XC25" s="11"/>
+      <c r="XD25" s="11"/>
+      <c r="XE25" s="11"/>
+      <c r="XF25" s="11"/>
+      <c r="XG25" s="11"/>
+      <c r="XH25" s="11"/>
+      <c r="XI25" s="11"/>
+      <c r="XJ25" s="11"/>
+      <c r="XK25" s="11"/>
+      <c r="XL25" s="11"/>
+      <c r="XM25" s="11"/>
+      <c r="XN25" s="11"/>
+      <c r="XO25" s="11"/>
+      <c r="XP25" s="11"/>
+      <c r="XQ25" s="11"/>
+      <c r="XR25" s="11"/>
+      <c r="XS25" s="11"/>
+      <c r="XT25" s="11"/>
+      <c r="XU25" s="11"/>
+      <c r="XV25" s="11"/>
+      <c r="XW25" s="11"/>
+      <c r="XX25" s="11"/>
+      <c r="XY25" s="11"/>
+      <c r="XZ25" s="11"/>
+      <c r="YA25" s="11"/>
+      <c r="YB25" s="11"/>
+      <c r="YC25" s="11"/>
+      <c r="YD25" s="11"/>
+      <c r="YE25" s="11"/>
+      <c r="YF25" s="11"/>
+      <c r="YG25" s="11"/>
+      <c r="YH25" s="11"/>
+      <c r="YI25" s="11"/>
+      <c r="YJ25" s="11"/>
+      <c r="YK25" s="11"/>
+      <c r="YL25" s="11"/>
+      <c r="YM25" s="11"/>
+      <c r="YN25" s="11"/>
+      <c r="YO25" s="11"/>
+      <c r="YP25" s="11"/>
+      <c r="YQ25" s="11"/>
+      <c r="YR25" s="11"/>
+      <c r="YS25" s="11"/>
+      <c r="YT25" s="11"/>
+      <c r="YU25" s="11"/>
+      <c r="YV25" s="11"/>
+      <c r="YW25" s="11"/>
+      <c r="YX25" s="11"/>
+      <c r="YY25" s="11"/>
+      <c r="YZ25" s="11"/>
+      <c r="ZA25" s="11"/>
+      <c r="ZB25" s="11"/>
+      <c r="ZC25" s="11"/>
+      <c r="ZD25" s="11"/>
+      <c r="ZE25" s="11"/>
+      <c r="ZF25" s="11"/>
+      <c r="ZG25" s="11"/>
+      <c r="ZH25" s="11"/>
+      <c r="ZI25" s="11"/>
+      <c r="ZJ25" s="11"/>
+      <c r="ZK25" s="11"/>
+      <c r="ZL25" s="11"/>
+      <c r="ZM25" s="11"/>
+      <c r="ZN25" s="11"/>
+      <c r="ZO25" s="11"/>
+      <c r="ZP25" s="11"/>
+      <c r="ZQ25" s="11"/>
+      <c r="ZR25" s="11"/>
+      <c r="ZS25" s="11"/>
+      <c r="ZT25" s="11"/>
+      <c r="ZU25" s="11"/>
+      <c r="ZV25" s="11"/>
+      <c r="ZW25" s="11"/>
+      <c r="ZX25" s="11"/>
+      <c r="ZY25" s="11"/>
+      <c r="ZZ25" s="11"/>
+      <c r="AAA25" s="11"/>
+      <c r="AAB25" s="11"/>
+      <c r="AAC25" s="11"/>
+      <c r="AAD25" s="11"/>
+      <c r="AAE25" s="11"/>
+      <c r="AAF25" s="11"/>
+      <c r="AAG25" s="11"/>
+      <c r="AAH25" s="11"/>
+      <c r="AAI25" s="11"/>
+      <c r="AAJ25" s="11"/>
+      <c r="AAK25" s="11"/>
+      <c r="AAL25" s="11"/>
+      <c r="AAM25" s="11"/>
+      <c r="AAN25" s="11"/>
+      <c r="AAO25" s="11"/>
+      <c r="AAP25" s="11"/>
+      <c r="AAQ25" s="11"/>
+      <c r="AAR25" s="11"/>
+      <c r="AAS25" s="11"/>
+      <c r="AAT25" s="11"/>
+      <c r="AAU25" s="11"/>
+      <c r="AAV25" s="11"/>
+      <c r="AAW25" s="11"/>
+      <c r="AAX25" s="11"/>
+      <c r="AAY25" s="11"/>
+      <c r="AAZ25" s="11"/>
+      <c r="ABA25" s="11"/>
+      <c r="ABB25" s="11"/>
+      <c r="ABC25" s="11"/>
+      <c r="ABD25" s="11"/>
+      <c r="ABE25" s="11"/>
+      <c r="ABF25" s="11"/>
+      <c r="ABG25" s="11"/>
+      <c r="ABH25" s="11"/>
+      <c r="ABI25" s="11"/>
+      <c r="ABJ25" s="11"/>
+      <c r="ABK25" s="11"/>
+      <c r="ABL25" s="11"/>
+      <c r="ABM25" s="11"/>
+      <c r="ABN25" s="11"/>
+      <c r="ABO25" s="11"/>
+      <c r="ABP25" s="11"/>
+      <c r="ABQ25" s="11"/>
+      <c r="ABR25" s="11"/>
+      <c r="ABS25" s="11"/>
+      <c r="ABT25" s="11"/>
+      <c r="ABU25" s="11"/>
+      <c r="ABV25" s="11"/>
+      <c r="ABW25" s="11"/>
+      <c r="ABX25" s="11"/>
+      <c r="ABY25" s="11"/>
+      <c r="ABZ25" s="11"/>
+      <c r="ACA25" s="11"/>
+      <c r="ACB25" s="11"/>
+      <c r="ACC25" s="11"/>
+      <c r="ACD25" s="11"/>
+      <c r="ACE25" s="11"/>
+      <c r="ACF25" s="11"/>
+      <c r="ACG25" s="11"/>
+      <c r="ACH25" s="11"/>
+      <c r="ACI25" s="11"/>
+      <c r="ACJ25" s="11"/>
+      <c r="ACK25" s="11"/>
+      <c r="ACL25" s="11"/>
+      <c r="ACM25" s="11"/>
+      <c r="ACN25" s="11"/>
+      <c r="ACO25" s="11"/>
+      <c r="ACP25" s="11"/>
+      <c r="ACQ25" s="11"/>
+      <c r="ACR25" s="11"/>
+      <c r="ACS25" s="11"/>
+      <c r="ACT25" s="11"/>
+      <c r="ACU25" s="11"/>
+      <c r="ACV25" s="11"/>
+      <c r="ACW25" s="11"/>
+      <c r="ACX25" s="11"/>
+      <c r="ACY25" s="11"/>
+      <c r="ACZ25" s="11"/>
+      <c r="ADA25" s="11"/>
+      <c r="ADB25" s="11"/>
+      <c r="ADC25" s="11"/>
+      <c r="ADD25" s="11"/>
+      <c r="ADE25" s="11"/>
+      <c r="ADF25" s="11"/>
+      <c r="ADG25" s="11"/>
+      <c r="ADH25" s="11"/>
+      <c r="ADI25" s="11"/>
+      <c r="ADJ25" s="11"/>
+      <c r="ADK25" s="11"/>
+      <c r="ADL25" s="11"/>
+      <c r="ADM25" s="11"/>
+      <c r="ADN25" s="11"/>
+      <c r="ADO25" s="11"/>
+      <c r="ADP25" s="11"/>
+      <c r="ADQ25" s="11"/>
+      <c r="ADR25" s="11"/>
+      <c r="ADS25" s="11"/>
+      <c r="ADT25" s="11"/>
+      <c r="ADU25" s="11"/>
+      <c r="ADV25" s="11"/>
+      <c r="ADW25" s="11"/>
+      <c r="ADX25" s="11"/>
+      <c r="ADY25" s="11"/>
+      <c r="ADZ25" s="11"/>
+      <c r="AEA25" s="11"/>
+      <c r="AEB25" s="11"/>
+      <c r="AEC25" s="11"/>
+      <c r="AED25" s="11"/>
+      <c r="AEE25" s="11"/>
+      <c r="AEF25" s="11"/>
+      <c r="AEG25" s="11"/>
+      <c r="AEH25" s="11"/>
+      <c r="AEI25" s="11"/>
+      <c r="AEJ25" s="11"/>
+      <c r="AEK25" s="11"/>
+      <c r="AEL25" s="11"/>
+      <c r="AEM25" s="11"/>
+      <c r="AEN25" s="11"/>
+      <c r="AEO25" s="11"/>
+      <c r="AEP25" s="11"/>
+      <c r="AEQ25" s="11"/>
+      <c r="AER25" s="11"/>
+      <c r="AES25" s="11"/>
+      <c r="AET25" s="11"/>
+      <c r="AEU25" s="11"/>
+      <c r="AEV25" s="11"/>
+      <c r="AEW25" s="11"/>
+      <c r="AEX25" s="11"/>
+      <c r="AEY25" s="11"/>
+      <c r="AEZ25" s="11"/>
+      <c r="AFA25" s="11"/>
+      <c r="AFB25" s="11"/>
+      <c r="AFC25" s="11"/>
+      <c r="AFD25" s="11"/>
+      <c r="AFE25" s="11"/>
+      <c r="AFF25" s="11"/>
+      <c r="AFG25" s="11"/>
+      <c r="AFH25" s="11"/>
+      <c r="AFI25" s="11"/>
+      <c r="AFJ25" s="11"/>
+      <c r="AFK25" s="11"/>
+      <c r="AFL25" s="11"/>
+      <c r="AFM25" s="11"/>
+      <c r="AFN25" s="11"/>
+      <c r="AFO25" s="11"/>
+      <c r="AFP25" s="11"/>
+      <c r="AFQ25" s="11"/>
+      <c r="AFR25" s="11"/>
+      <c r="AFS25" s="11"/>
+      <c r="AFT25" s="11"/>
+      <c r="AFU25" s="11"/>
+      <c r="AFV25" s="11"/>
+      <c r="AFW25" s="11"/>
+      <c r="AFX25" s="11"/>
+      <c r="AFY25" s="11"/>
+      <c r="AFZ25" s="11"/>
+      <c r="AGA25" s="11"/>
+      <c r="AGB25" s="11"/>
+      <c r="AGC25" s="11"/>
+      <c r="AGD25" s="11"/>
+      <c r="AGE25" s="11"/>
+      <c r="AGF25" s="11"/>
+      <c r="AGG25" s="11"/>
+      <c r="AGH25" s="11"/>
+      <c r="AGI25" s="11"/>
+      <c r="AGJ25" s="11"/>
+      <c r="AGK25" s="11"/>
+      <c r="AGL25" s="11"/>
+      <c r="AGM25" s="11"/>
+      <c r="AGN25" s="11"/>
+      <c r="AGO25" s="11"/>
+      <c r="AGP25" s="11"/>
+      <c r="AGQ25" s="11"/>
+      <c r="AGR25" s="11"/>
+      <c r="AGS25" s="11"/>
+      <c r="AGT25" s="11"/>
+      <c r="AGU25" s="11"/>
+      <c r="AGV25" s="11"/>
+      <c r="AGW25" s="11"/>
+      <c r="AGX25" s="11"/>
+      <c r="AGY25" s="11"/>
+      <c r="AGZ25" s="11"/>
+      <c r="AHA25" s="11"/>
+      <c r="AHB25" s="11"/>
+      <c r="AHC25" s="11"/>
+      <c r="AHD25" s="11"/>
+      <c r="AHE25" s="11"/>
+      <c r="AHF25" s="11"/>
+      <c r="AHG25" s="11"/>
+      <c r="AHH25" s="11"/>
+      <c r="AHI25" s="11"/>
+      <c r="AHJ25" s="11"/>
+      <c r="AHK25" s="11"/>
+      <c r="AHL25" s="11"/>
+      <c r="AHM25" s="11"/>
+      <c r="AHN25" s="11"/>
+      <c r="AHO25" s="11"/>
+      <c r="AHP25" s="11"/>
+      <c r="AHQ25" s="11"/>
+      <c r="AHR25" s="11"/>
+      <c r="AHS25" s="11"/>
+      <c r="AHT25" s="11"/>
+      <c r="AHU25" s="11"/>
+      <c r="AHV25" s="11"/>
+      <c r="AHW25" s="11"/>
+      <c r="AHX25" s="11"/>
+      <c r="AHY25" s="11"/>
+      <c r="AHZ25" s="11"/>
+      <c r="AIA25" s="11"/>
+      <c r="AIB25" s="11"/>
+      <c r="AIC25" s="11"/>
+      <c r="AID25" s="11"/>
+      <c r="AIE25" s="11"/>
+      <c r="AIF25" s="11"/>
+      <c r="AIG25" s="11"/>
+      <c r="AIH25" s="11"/>
+      <c r="AII25" s="11"/>
+      <c r="AIJ25" s="11"/>
+      <c r="AIK25" s="11"/>
+      <c r="AIL25" s="11"/>
+      <c r="AIM25" s="11"/>
+      <c r="AIN25" s="11"/>
+      <c r="AIO25" s="11"/>
+      <c r="AIP25" s="11"/>
+      <c r="AIQ25" s="11"/>
+      <c r="AIR25" s="11"/>
+      <c r="AIS25" s="11"/>
+      <c r="AIT25" s="11"/>
+      <c r="AIU25" s="11"/>
+      <c r="AIV25" s="11"/>
+      <c r="AIW25" s="11"/>
+      <c r="AIX25" s="11"/>
+      <c r="AIY25" s="11"/>
+      <c r="AIZ25" s="11"/>
+      <c r="AJA25" s="11"/>
+      <c r="AJB25" s="11"/>
+      <c r="AJC25" s="11"/>
+      <c r="AJD25" s="11"/>
+      <c r="AJE25" s="11"/>
+      <c r="AJF25" s="11"/>
+      <c r="AJG25" s="11"/>
+      <c r="AJH25" s="11"/>
+      <c r="AJI25" s="11"/>
+      <c r="AJJ25" s="11"/>
+      <c r="AJK25" s="11"/>
+      <c r="AJL25" s="11"/>
+      <c r="AJM25" s="11"/>
+      <c r="AJN25" s="11"/>
+      <c r="AJO25" s="11"/>
+      <c r="AJP25" s="11"/>
+      <c r="AJQ25" s="11"/>
+      <c r="AJR25" s="11"/>
+      <c r="AJS25" s="11"/>
+      <c r="AJT25" s="11"/>
+      <c r="AJU25" s="11"/>
+      <c r="AJV25" s="11"/>
+      <c r="AJW25" s="11"/>
+      <c r="AJX25" s="11"/>
+      <c r="AJY25" s="11"/>
+      <c r="AJZ25" s="11"/>
+      <c r="AKA25" s="11"/>
+      <c r="AKB25" s="11"/>
+      <c r="AKC25" s="11"/>
+      <c r="AKD25" s="11"/>
+      <c r="AKE25" s="11"/>
+      <c r="AKF25" s="11"/>
+      <c r="AKG25" s="11"/>
+      <c r="AKH25" s="11"/>
+      <c r="AKI25" s="11"/>
+      <c r="AKJ25" s="11"/>
+      <c r="AKK25" s="11"/>
+      <c r="AKL25" s="11"/>
+      <c r="AKM25" s="11"/>
+      <c r="AKN25" s="11"/>
+      <c r="AKO25" s="11"/>
+      <c r="AKP25" s="11"/>
+      <c r="AKQ25" s="11"/>
+      <c r="AKR25" s="11"/>
+      <c r="AKS25" s="11"/>
+      <c r="AKT25" s="11"/>
+      <c r="AKU25" s="11"/>
+      <c r="AKV25" s="11"/>
+      <c r="AKW25" s="11"/>
+      <c r="AKX25" s="11"/>
+      <c r="AKY25" s="11"/>
+      <c r="AKZ25" s="11"/>
+      <c r="ALA25" s="11"/>
+      <c r="ALB25" s="11"/>
+      <c r="ALC25" s="11"/>
+      <c r="ALD25" s="11"/>
+      <c r="ALE25" s="11"/>
+      <c r="ALF25" s="11"/>
+      <c r="ALG25" s="11"/>
+      <c r="ALH25" s="11"/>
+      <c r="ALI25" s="11"/>
+      <c r="ALJ25" s="11"/>
+      <c r="ALK25" s="11"/>
+      <c r="ALL25" s="11"/>
+      <c r="ALM25" s="11"/>
+      <c r="ALN25" s="11"/>
+      <c r="ALO25" s="11"/>
+      <c r="ALP25" s="11"/>
+      <c r="ALQ25" s="11"/>
+      <c r="ALR25" s="11"/>
+      <c r="ALS25" s="11"/>
+      <c r="ALT25" s="11"/>
+      <c r="ALU25" s="11"/>
+      <c r="ALV25" s="11"/>
+      <c r="ALW25" s="11"/>
+      <c r="ALX25" s="11"/>
+      <c r="ALY25" s="11"/>
+      <c r="ALZ25" s="11"/>
+      <c r="AMA25" s="11"/>
+      <c r="AMB25" s="11"/>
+      <c r="AMC25" s="11"/>
+      <c r="AMD25" s="11"/>
+      <c r="AME25" s="11"/>
+      <c r="AMF25" s="11"/>
+      <c r="AMG25" s="11"/>
+      <c r="AMH25" s="11"/>
+      <c r="AMI25" s="11"/>
+      <c r="AMJ25" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>

</xml_diff>

<commit_message>
- Thêm mô tả homepage trong SDD - Update báo cáo cá nhân của Thành
</commit_message>
<xml_diff>
--- a/BaoCaoCaNhan/Weekly_Report_Thanh.xlsx
+++ b/BaoCaoCaNhan/Weekly_Report_Thanh.xlsx
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>Project</t>
   </si>
@@ -604,11 +604,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3135,7 +3135,7 @@
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3172,10 +3172,10 @@
         <v>34</v>
       </c>
       <c r="E1" s="1"/>
-      <c r="F1" s="14">
+      <c r="F1" s="15">
         <v>50902476</v>
       </c>
-      <c r="G1" s="14"/>
+      <c r="G1" s="15"/>
       <c r="P1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" s="12" customFormat="1">
+    <row r="4" spans="1:1024" s="12" customFormat="1" ht="42.75">
       <c r="A4" s="8">
         <v>41099</v>
       </c>
@@ -8452,7 +8452,7 @@
       <c r="AMJ8" s="11"/>
     </row>
     <row r="9" spans="1:1024" s="12" customFormat="1" ht="28.5">
-      <c r="A9" s="15">
+      <c r="A9" s="14">
         <v>40918</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -8461,11 +8461,15 @@
       <c r="C9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="E9" s="9">
         <v>4</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="9">
+        <v>3.5</v>
+      </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -25953,8 +25957,8 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
       <c r="P1" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>